<commit_message>
progetto linguaggi parte B, completata relazione, espansa error correction
</commit_message>
<xml_diff>
--- a/Bruniera/linguaggi e compilatori/progetto/parteB/esecuzione slr.xlsx
+++ b/Bruniera/linguaggi e compilatori/progetto/parteB/esecuzione slr.xlsx
@@ -13,9 +13,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="51">
-  <si>
-    <t xml:space="preserve">cases id + id { id s cases id id ) { id s } s }</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="71">
+  <si>
+    <t xml:space="preserve">cases id + id { id s cases id id ) { id s } s } $</t>
   </si>
   <si>
     <t>s3</t>
@@ -24,7 +24,7 @@
     <t xml:space="preserve">0 cases 3</t>
   </si>
   <si>
-    <t xml:space="preserve">id + id { id s cases id id ) { id s } s }</t>
+    <t xml:space="preserve">id + id { id s cases id id ) { id s } s } $</t>
   </si>
   <si>
     <t>s7</t>
@@ -33,7 +33,7 @@
     <t xml:space="preserve">0 cases 3 id 7</t>
   </si>
   <si>
-    <t xml:space="preserve">+ id { id s cases id id ) { id s } s }</t>
+    <t xml:space="preserve">+ id { id s cases id id ) { id s } s } $</t>
   </si>
   <si>
     <t>L-&gt;id</t>
@@ -54,13 +54,13 @@
     <t xml:space="preserve">0 cases 3 E 4 + 9</t>
   </si>
   <si>
-    <t xml:space="preserve">id { id s cases id id ) { id s } s }</t>
+    <t xml:space="preserve">id { id s cases id id ) { id s } s } $</t>
   </si>
   <si>
     <t xml:space="preserve">0 cases 3 E 4 + 9 id 7</t>
   </si>
   <si>
-    <t xml:space="preserve">{ id s cases id id ) { id s } s }</t>
+    <t xml:space="preserve">{ id s cases id id ) { id s } s } $</t>
   </si>
   <si>
     <t xml:space="preserve">0 cases 3 E 4 + 9 L 5</t>
@@ -78,7 +78,7 @@
     <t xml:space="preserve">0 cases 3 E 4 { 8</t>
   </si>
   <si>
-    <t xml:space="preserve">id s cases id id ) { id s } s }</t>
+    <t xml:space="preserve">id s cases id id ) { id s } s } $</t>
   </si>
   <si>
     <t>s13</t>
@@ -87,7 +87,7 @@
     <t xml:space="preserve">0 cases 3 E 4 { 8 id 13</t>
   </si>
   <si>
-    <t xml:space="preserve">s cases id id ) { id s } s }</t>
+    <t xml:space="preserve">s cases id id ) { id s } s } $</t>
   </si>
   <si>
     <t>s2</t>
@@ -96,73 +96,133 @@
     <t xml:space="preserve">0 cases 3 E 4 { 8 id 13 s 2</t>
   </si>
   <si>
-    <t xml:space="preserve">cases id id ) { id s } s }</t>
-  </si>
-  <si>
-    <t xml:space="preserve">double statement</t>
-  </si>
-  <si>
-    <t xml:space="preserve">id id ) { id s } s }</t>
-  </si>
-  <si>
-    <t>S-&gt;s</t>
+    <t xml:space="preserve">cases id id ) { id s } s } $</t>
+  </si>
+  <si>
+    <t xml:space="preserve">unexpected cases, accepting anyway, S-&gt;s</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0 cases 3 E 4 { 8 id 13 S 18</t>
+  </si>
+  <si>
+    <t xml:space="preserve">S-&gt;s </t>
   </si>
   <si>
     <t xml:space="preserve">0 cases 3 E 4 { 8 id 13 S 18 </t>
   </si>
   <si>
+    <t xml:space="preserve">missing id</t>
+  </si>
+  <si>
     <t xml:space="preserve">0 cases 3 E 4 { 8 id 13 S 18 id 13</t>
   </si>
   <si>
-    <t xml:space="preserve">id ) { id s } s }</t>
+    <t xml:space="preserve">0 cases 3 E 4 { 8 id 13 S 18 id 13 cases 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">id id ) { id s } s } $</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0 cases 3 E 4 { 8 id 13 S 18 id 13 cases 3 id 7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">id ) { id s } s } $</t>
   </si>
   <si>
     <t xml:space="preserve">unexpected id</t>
   </si>
   <si>
-    <t xml:space="preserve">s } s }</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0 cases 3 E 4 { 8 id 13 S 18 id 13 s 2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">} s }</t>
+    <t xml:space="preserve">) { id s } s } $</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0 cases 3 E 4 { 8 id 13 S 18 id 13 cases 3 L 5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0 cases 3 E 4 { 8 id 13 S 18 id 13 cases 3 E 4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">unexpected )</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{ id s } s } $</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0 cases 3 E 4 { 8 id 13 S 18 id 13 cases 3 E 4 { 8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">id s } s } $</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0 cases 3 E 4 { 8 id 13 S 18 id 13 cases 3 E 4 { 8 id 13</t>
+  </si>
+  <si>
+    <t xml:space="preserve">s } s } $</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0 cases 3 E 4 { 8 id 13 S 18 id 13 cases 3 E 4 { 8 id 13 s 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">} s } $</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0 cases 3 E 4 { 8 id 13 S 18 id 13 cases 3 E 4 { 8 id 13 S 18</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A-&gt;id S</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0 cases 3 E 4 { 8 id 13 S 18 id 13 cases 3 E 4 { 8 A 12</t>
+  </si>
+  <si>
+    <t>s17</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0 cases 3 E 4 { 8 id 13 S 18 id 13 cases 3 E 4 { 8 A 12 } 17</t>
+  </si>
+  <si>
+    <t xml:space="preserve">s } $</t>
+  </si>
+  <si>
+    <t xml:space="preserve">unexpected cases, accepting anyway, S-&gt;cases E { A }</t>
   </si>
   <si>
     <t xml:space="preserve">0 cases 3 E 4 { 8 id 13 S 18 id 13 S 18</t>
   </si>
   <si>
-    <t xml:space="preserve">A-&gt;id S</t>
+    <t xml:space="preserve">0 cases 3 E 4 { 8 id 13 S 18 id 13 S 18 id 13</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0 cases 3 E 4 { 8 id 13 S 18 id 13 S 18 id 13 s 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">} $</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0 cases 3 E 4 { 8 id 13 S 18 id 13 S 18 id 13 S 18</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0 cases 3 E 4 { 8 id 13 S 18 id 13 S 18 A 19</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A-&gt;id S A</t>
   </si>
   <si>
     <t xml:space="preserve">0 cases 3 E 4 { 8 id 13 S 18 A 19</t>
   </si>
   <si>
-    <t xml:space="preserve">A-&gt;id S A</t>
-  </si>
-  <si>
     <t xml:space="preserve">0 cases 3 E 4 { 8 A 12</t>
   </si>
   <si>
-    <t>s17</t>
-  </si>
-  <si>
     <t xml:space="preserve">0 cases 3 E 4 { 8 A 12 } 17</t>
   </si>
   <si>
-    <t xml:space="preserve">s }</t>
-  </si>
-  <si>
-    <t xml:space="preserve">unexpected s</t>
+    <t>$</t>
+  </si>
+  <si>
+    <t xml:space="preserve">S-&gt;cases E { A }</t>
   </si>
   <si>
     <t xml:space="preserve">0 S 1</t>
-  </si>
-  <si>
-    <t>}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">unexpected }</t>
   </si>
   <si>
     <t>Acc</t>
@@ -254,24 +314,21 @@
     <xf fontId="2" fillId="3" borderId="0" numFmtId="0" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="0"/>
     <xf fontId="3" fillId="4" borderId="0" numFmtId="0" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="0" fillId="0" borderId="1" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf fontId="0" fillId="0" borderId="1" numFmtId="0" xfId="0" applyBorder="1"/>
-    <xf fontId="0" fillId="0" borderId="1" numFmtId="0" xfId="0" applyBorder="1"/>
-    <xf fontId="0" fillId="0" borderId="1" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf fontId="1" fillId="2" borderId="1" numFmtId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf fontId="0" fillId="0" borderId="1" numFmtId="0" xfId="0" applyBorder="1">
       <protection hidden="0" locked="1"/>
     </xf>
+    <xf fontId="2" fillId="3" borderId="1" numFmtId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf fontId="0" fillId="0" borderId="1" numFmtId="0" xfId="0" applyBorder="1"/>
     <xf fontId="0" fillId="0" borderId="1" numFmtId="0" xfId="0" applyBorder="1">
       <protection hidden="0" locked="1"/>
     </xf>
-    <xf fontId="2" fillId="3" borderId="1" numFmtId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf fontId="3" fillId="4" borderId="1" numFmtId="0" xfId="3" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="4">
@@ -783,13 +840,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
   <sheetViews>
-    <sheetView zoomScale="100" workbookViewId="0">
+    <sheetView topLeftCell="A22" zoomScale="100" workbookViewId="0">
       <selection activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="31.57421875"/>
+    <col customWidth="1" min="1" max="1" width="48.140625"/>
     <col customWidth="1" min="2" max="2" width="35.00390625"/>
     <col customWidth="1" min="3" max="3" width="16.28125"/>
   </cols>
@@ -801,29 +858,29 @@
       <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="2" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" ht="14.25">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="2" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="3" ht="14.25">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="C3" s="3" t="s">
         <v>7</v>
       </c>
     </row>
@@ -831,10 +888,10 @@
       <c r="A4" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="C4" s="3" t="s">
         <v>9</v>
       </c>
     </row>
@@ -842,10 +899,10 @@
       <c r="A5" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="7" t="s">
+      <c r="B5" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="2" t="s">
         <v>11</v>
       </c>
     </row>
@@ -856,7 +913,7 @@
       <c r="B6" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C6" s="2" t="s">
         <v>4</v>
       </c>
     </row>
@@ -864,10 +921,10 @@
       <c r="A7" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C7" s="5" t="s">
+      <c r="C7" s="3" t="s">
         <v>7</v>
       </c>
     </row>
@@ -875,10 +932,10 @@
       <c r="A8" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B8" s="6" t="s">
+      <c r="B8" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="C8" s="5" t="s">
+      <c r="C8" s="3" t="s">
         <v>9</v>
       </c>
     </row>
@@ -886,10 +943,10 @@
       <c r="A9" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B9" s="6" t="s">
+      <c r="B9" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="C9" s="5" t="s">
+      <c r="C9" s="3" t="s">
         <v>18</v>
       </c>
     </row>
@@ -897,10 +954,10 @@
       <c r="A10" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B10" s="7" t="s">
+      <c r="B10" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="C10" s="3" t="s">
+      <c r="C10" s="2" t="s">
         <v>19</v>
       </c>
     </row>
@@ -911,7 +968,7 @@
       <c r="B11" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C11" s="3" t="s">
+      <c r="C11" s="2" t="s">
         <v>22</v>
       </c>
     </row>
@@ -933,18 +990,18 @@
       <c r="B13" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="C13" s="8" t="s">
+      <c r="C13" s="5" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="14" ht="14.25">
-      <c r="A14" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="B14" s="3" t="s">
+      <c r="A14" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="C14" s="5" t="s">
+      <c r="B14" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="C14" s="3" t="s">
         <v>30</v>
       </c>
     </row>
@@ -952,108 +1009,253 @@
       <c r="A15" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B15" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>22</v>
+      <c r="B15" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="16" ht="14.25">
       <c r="A16" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="B16" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="C16" s="8" t="s">
+      <c r="B16" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="C16" s="6" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" ht="14.25">
+      <c r="A17" s="6" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="17" ht="14.25">
-      <c r="A17" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="B17" s="2" t="s">
+      <c r="B17" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="C17" s="2" t="s">
-        <v>25</v>
+      <c r="C17" s="6" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="18" ht="14.25">
-      <c r="A18" s="2" t="s">
+      <c r="A18" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="B18" s="3" t="s">
+      <c r="B18" s="6" t="s">
         <v>37</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>30</v>
+        <v>38</v>
       </c>
     </row>
     <row r="19" ht="14.25">
       <c r="A19" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="B19" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="C19" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="B19" s="4" t="s">
         <v>39</v>
       </c>
+      <c r="C19" s="3" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="20" ht="14.25">
-      <c r="A20" s="2" t="s">
+      <c r="A20" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="B20" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="C20" s="5" t="s">
+      <c r="B20" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="21" ht="14.25">
+      <c r="A21" s="6" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="21" ht="14.25">
-      <c r="A21" s="2" t="s">
+      <c r="B21" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="C21" s="5" t="s">
         <v>42</v>
-      </c>
-      <c r="B21" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="C21" s="3" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="22" ht="14.25">
       <c r="A22" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B22" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="C22" s="6" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="23" ht="14.25">
+      <c r="A23" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="B22" s="7" t="s">
+      <c r="B23" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="C22" s="3" t="s">
+      <c r="C23" s="6" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="24" ht="14.25">
+      <c r="A24" s="6" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="23" ht="14.25">
-      <c r="A23" s="2" t="s">
+      <c r="B24" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="B23" s="7" t="s">
+      <c r="C24" s="6" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="25" ht="14.25">
+      <c r="A25" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="C23" s="3" t="s">
+      <c r="B25" s="2" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="24" ht="14.25">
-      <c r="A24" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="B24" s="3"/>
-      <c r="C24" s="9" t="s">
+      <c r="C25" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="26" ht="14.25">
+      <c r="A26" s="6" t="s">
         <v>50</v>
+      </c>
+      <c r="B26" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="27" ht="14.25">
+      <c r="A27" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="B27" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="28" ht="14.25">
+      <c r="A28" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="C28" s="5" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="29" ht="14.25">
+      <c r="A29" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="B29" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="C29" s="5" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="30" ht="14.25">
+      <c r="A30" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="B30" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="31" ht="14.25">
+      <c r="A31" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="32" ht="14.25">
+      <c r="A32" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="B32" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="C32" s="3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="33" ht="14.25">
+      <c r="A33" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="B33" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="C33" s="3" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="34" ht="14.25">
+      <c r="A34" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="B34" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="C34" s="3" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="35" ht="14.25">
+      <c r="A35" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="B35" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="36" ht="14.25">
+      <c r="A36" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="C36" s="3" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="37" ht="14.25">
+      <c r="A37" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="C37" s="8" t="s">
+        <v>70</v>
       </c>
     </row>
   </sheetData>

</xml_diff>